<commit_message>
inital config filter done
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2033660D-01C1-4F34-897C-A7D8C59BDE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8B8201-FF67-4AE0-9727-46EFEAB67233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,9 +168,6 @@
     <t>q</t>
   </si>
   <si>
-    <t>APAC</t>
-  </si>
-  <si>
     <t>LAN_IP+mask</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>tritri</t>
+  </si>
+  <si>
+    <t>NAM</t>
   </si>
 </sst>
 </file>
@@ -709,7 +709,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -801,6 +801,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -819,19 +828,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1115,7 +1114,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,10 +1126,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="37"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
         <v>17</v>
@@ -1141,7 +1140,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>44</v>
@@ -1155,14 +1154,14 @@
       <c r="B3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="41"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="27"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="4"/>
       <c r="D4" s="20"/>
     </row>
@@ -1173,7 +1172,7 @@
       <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="42"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1183,7 +1182,7 @@
       <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="43"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1203,7 +1202,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>44</v>
@@ -1223,10 +1222,10 @@
       <c r="D9" s="23"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="36"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="4"/>
       <c r="D10" s="24"/>
     </row>
@@ -1237,7 +1236,7 @@
       <c r="B11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="42"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="21" t="s">
         <v>18</v>
       </c>
@@ -1249,9 +1248,9 @@
       <c r="B12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="43"/>
+      <c r="C12" s="33"/>
       <c r="D12" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1261,7 +1260,7 @@
       <c r="B13" s="8">
         <v>100</v>
       </c>
-      <c r="C13" s="43"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="22" t="s">
         <v>20</v>
       </c>
@@ -1273,7 +1272,7 @@
       <c r="B14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="43"/>
+      <c r="C14" s="33"/>
       <c r="D14" s="22"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1283,7 +1282,7 @@
       <c r="B15" s="8">
         <v>20</v>
       </c>
-      <c r="C15" s="43"/>
+      <c r="C15" s="33"/>
       <c r="D15" s="22" t="s">
         <v>20</v>
       </c>
@@ -1301,13 +1300,13 @@
       <c r="D16" s="25"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="36"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="4"/>
       <c r="D17" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1317,7 +1316,7 @@
       <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="42"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="21"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1325,7 +1324,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="43"/>
+      <c r="C19" s="33"/>
       <c r="D19" s="22" t="s">
         <v>19</v>
       </c>
@@ -1337,7 +1336,7 @@
       <c r="B20" s="8">
         <v>40</v>
       </c>
-      <c r="C20" s="43"/>
+      <c r="C20" s="33"/>
       <c r="D20" s="22"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1347,7 +1346,7 @@
       <c r="B21" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="43"/>
+      <c r="C21" s="33"/>
       <c r="D21" s="22"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1357,7 +1356,7 @@
       <c r="B22" s="8">
         <v>20</v>
       </c>
-      <c r="C22" s="43"/>
+      <c r="C22" s="33"/>
       <c r="D22" s="22"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1373,10 +1372,10 @@
       <c r="D23" s="25"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="36"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="13"/>
       <c r="D24" s="26"/>
     </row>
@@ -1399,7 +1398,7 @@
       <c r="B26" s="8">
         <v>50</v>
       </c>
-      <c r="C26" s="43"/>
+      <c r="C26" s="33"/>
       <c r="D26" s="22"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1409,14 +1408,14 @@
       <c r="B27" s="15">
         <v>40</v>
       </c>
-      <c r="C27" s="41"/>
+      <c r="C27" s="31"/>
       <c r="D27" s="25"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="38"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="4"/>
       <c r="D28" s="24"/>
     </row>
@@ -1427,27 +1426,27 @@
       <c r="B29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="42"/>
+      <c r="C29" s="32"/>
       <c r="D29" s="21"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="41"/>
+      <c r="C30" s="31"/>
       <c r="D30" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B7" xr:uid="{6F22417C-AD18-4E4D-B071-70A75C435361}">
@@ -1486,45 +1485,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="39"/>
+      <c r="A1" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="42"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="40">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="42"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="39"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="40">
-        <v>2</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="39"/>
+      <c r="B5" s="42"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1532,7 +1531,7 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1556,22 +1555,22 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="42"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="39"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="B2" s="42"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="39"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="39"/>
+      <c r="B3" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
function get initial string renamed to get region string.
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8B8201-FF67-4AE0-9727-46EFEAB67233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDB95E4-5DF2-4E7A-9CE0-BB440F88A105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>Region</t>
   </si>
@@ -81,9 +81,6 @@
     <t>DHCP</t>
   </si>
   <si>
-    <t>GW</t>
-  </si>
-  <si>
     <t>Explanatory notes</t>
   </si>
   <si>
@@ -202,6 +199,27 @@
   </si>
   <si>
     <t>NAM</t>
+  </si>
+  <si>
+    <t>APN</t>
+  </si>
+  <si>
+    <t>internet.odjosky.com</t>
+  </si>
+  <si>
+    <t>Backup_IP+mask</t>
+  </si>
+  <si>
+    <t>Main_GW</t>
+  </si>
+  <si>
+    <t>Backup_GW</t>
+  </si>
+  <si>
+    <t>Backup_port_speed</t>
+  </si>
+  <si>
+    <t>backup_DC_Tunnel_Speed</t>
   </si>
 </sst>
 </file>
@@ -279,7 +297,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -462,17 +480,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -597,19 +604,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -703,6 +697,17 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -714,114 +719,108 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -830,6 +829,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1111,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,44 +1131,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="35"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="30"/>
+      <c r="B2" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="27"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="39"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="20"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1172,8 +1177,8 @@
       <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="21"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1182,8 +1187,8 @@
       <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="22"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1192,65 +1197,65 @@
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="22"/>
+      <c r="C7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="22"/>
+        <v>47</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="23"/>
+      <c r="C9" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="21"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="41"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="24"/>
+      <c r="D10" s="22"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="21" t="s">
-        <v>18</v>
+      <c r="C11" s="29"/>
+      <c r="D11" s="19" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="22" t="s">
-        <v>47</v>
+        <v>22</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="20" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1260,20 +1265,20 @@
       <c r="B13" s="8">
         <v>100</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="22" t="s">
-        <v>20</v>
+      <c r="C13" s="30"/>
+      <c r="D13" s="20" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="22"/>
+        <v>25</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="20"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -1282,189 +1287,210 @@
       <c r="B15" s="8">
         <v>20</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="25"/>
+      <c r="D16" s="20"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="6" t="s">
+      <c r="A17" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="31"/>
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="21"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="22" t="s">
-        <v>19</v>
-      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="19"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="8">
-        <v>40</v>
-      </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="22"/>
+        <v>60</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="20" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="22"/>
+        <v>61</v>
+      </c>
+      <c r="B21" s="8">
+        <v>40</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="20"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="8">
+        <v>26</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="8">
         <v>20</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="22"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
+      <c r="C23" s="30"/>
+      <c r="D23" s="20"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="25"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="26"/>
+      <c r="D24" s="20"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="42"/>
+      <c r="D25" s="19"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="37"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="41"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="C27" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="19"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="B28" s="8">
+        <v>50</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="20"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="13">
+        <v>40</v>
+      </c>
+      <c r="C29" s="28"/>
+      <c r="D29" s="23"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="33"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="22"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="19"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="21"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="8">
-        <v>50</v>
-      </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="22"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="15">
-        <v>40</v>
-      </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="25"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="24"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="6" t="s">
+      <c r="B32" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="21"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="27"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A30:B30"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B7" xr:uid="{6F22417C-AD18-4E4D-B071-70A75C435361}">
       <formula1>"BASE,SMART,FLOW"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B8" xr:uid="{4F4D49CC-A654-4619-9B24-65BC6A1BEBDE}">
       <formula1>"False, True - New Router, True - Production router"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B16 B23 B9" xr:uid="{40737FED-04A3-4B54-B994-6B1C06BE492C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B9 B16 B24" xr:uid="{40737FED-04A3-4B54-B994-6B1C06BE492C}">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B25" xr:uid="{92AB63BB-4C2D-4BF2-85DE-EF3376E22321}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B27" xr:uid="{92AB63BB-4C2D-4BF2-85DE-EF3376E22321}">
       <formula1>"IPSEC,GRE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B2" xr:uid="{EE08AF00-27BF-4CFF-B4E8-48A38BCB5CAE}">
       <formula1>"APAC,EMEA,NAM"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" prompt="Select the cell to the left to activate the drop-down menu." sqref="C2 C16 C7:C9 C23 C25" xr:uid="{06058C94-713F-44F2-B256-641C730C7456}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" prompt="Select the cell to the left to activate the drop-down menu." sqref="C2 C16:C17 C7:C9 C24:C25 C27" xr:uid="{06058C94-713F-44F2-B256-641C730C7456}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B17 B25" xr:uid="{2DB65D46-00C2-4C0B-A067-155B441BF7B7}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1485,45 +1511,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="42"/>
+      <c r="A1" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="40"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="42"/>
+      <c r="A3" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="40"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="42"/>
+      <c r="A5" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="40"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1531,7 +1557,7 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1555,22 +1581,22 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="40"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="42"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="B2" s="40"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="42"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="42"/>
+      <c r="B3" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1597,22 +1623,22 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
file_ending_cleanup - match string needs to be fixed.
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A9B9E7-3E10-4198-B55A-481521CCAE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621E63F9-05B5-41DD-96B1-7DCA6D649E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -219,7 +219,7 @@
     <t>backup_DC_Tunnel_Speed</t>
   </si>
   <si>
-    <t>APAC</t>
+    <t>NAM</t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1119,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
file_ending_cleanup - the issue with filtering is fixed
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621E63F9-05B5-41DD-96B1-7DCA6D649E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95216D08-0D0A-4ED4-BDD7-F934487865D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -219,7 +219,7 @@
     <t>backup_DC_Tunnel_Speed</t>
   </si>
   <si>
-    <t>NAM</t>
+    <t>EMEA</t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1119,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
The cellular part of the code is exteneded so it also checks the backup link
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34894BB6-CBD8-4F01-A45C-EBBB653BC9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9BE7F3-BB5E-44A7-A489-40636EC0236F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1119,7 +1119,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,7 +1297,7 @@
         <v>42</v>
       </c>
       <c r="B16" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>43</v>
@@ -1379,7 +1379,7 @@
         <v>42</v>
       </c>
       <c r="B24" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Minor zscaler config change
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,15 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937B8736-360F-410B-9B93-611C91521977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D823F1D-F3F5-46F1-B399-71DA8324D97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Info" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
-    <sheet name="LAN routes" sheetId="2" r:id="rId4"/>
+    <sheet name="LAN routes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="BASE_SMART_FLOW">'Main Info'!$B$7:$B$8</definedName>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>Region</t>
   </si>
@@ -177,27 +175,6 @@
     <t>True - Production router</t>
   </si>
   <si>
-    <t>jedna</t>
-  </si>
-  <si>
-    <t>dva</t>
-  </si>
-  <si>
-    <t>tri</t>
-  </si>
-  <si>
-    <t>dvojka</t>
-  </si>
-  <si>
-    <t>Trojka</t>
-  </si>
-  <si>
-    <t>jednotka</t>
-  </si>
-  <si>
-    <t>tritri</t>
-  </si>
-  <si>
     <t>APN</t>
   </si>
   <si>
@@ -220,13 +197,22 @@
   </si>
   <si>
     <t>APAC</t>
+  </si>
+  <si>
+    <t>This means if you want the zscaler to be configured</t>
+  </si>
+  <si>
+    <t>Is Zscaler applicable?</t>
+  </si>
+  <si>
+    <t>If you select 4G+Cellular to TRUE APN has to be specified.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +250,12 @@
       <family val="1"/>
       <charset val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -297,7 +289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -705,6 +697,43 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -714,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -833,8 +862,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1116,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>43</v>
@@ -1248,7 +1289,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>22</v>
@@ -1306,13 +1347,15 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C17" s="31"/>
-      <c r="D17" s="21"/>
+      <c r="D17" s="21" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="40" t="s">
@@ -1326,17 +1369,19 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="29"/>
-      <c r="D19" s="19"/>
+      <c r="D19" s="19" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="30"/>
@@ -1346,7 +1391,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B21" s="8">
         <v>40</v>
@@ -1366,7 +1411,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B23" s="8">
         <v>20</v>
@@ -1388,10 +1433,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C25" s="33"/>
       <c r="D25" s="19"/>
@@ -1405,75 +1450,89 @@
       <c r="D26" s="32"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="C27" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B28" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C28" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="19"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="D28" s="19"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B29" s="8">
         <v>50</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="20"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
+      <c r="C29" s="30"/>
+      <c r="D29" s="20"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="13">
+      <c r="B30" s="13">
         <v>40</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="23"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34" t="s">
+      <c r="C30" s="28"/>
+      <c r="D30" s="23"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="22"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="B31" s="35"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="22"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="19"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
+      <c r="C32" s="29"/>
+      <c r="D32" s="19"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B33" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="24"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A26:B26"/>
   </mergeCells>
-  <dataValidations count="7">
+  <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B7" xr:uid="{6F22417C-AD18-4E4D-B071-70A75C435361}">
       <formula1>"BASE,SMART,FLOW"</formula1>
     </dataValidation>
@@ -1483,14 +1542,17 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B9 B16 B24" xr:uid="{40737FED-04A3-4B54-B994-6B1C06BE492C}">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B27" xr:uid="{92AB63BB-4C2D-4BF2-85DE-EF3376E22321}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B28" xr:uid="{92AB63BB-4C2D-4BF2-85DE-EF3376E22321}">
       <formula1>"IPSEC,GRE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B2" xr:uid="{EE08AF00-27BF-4CFF-B4E8-48A38BCB5CAE}">
       <formula1>"APAC,EMEA,NAM"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" prompt="Select the cell to the left to activate the drop-down menu." sqref="C2 C16:C17 C7:C9 C24:C25 C27" xr:uid="{06058C94-713F-44F2-B256-641C730C7456}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" prompt="Select the cell to the left to activate the drop-down menu." sqref="C2 C16:C17 C7:C9 C24:C25 C27:C28" xr:uid="{06058C94-713F-44F2-B256-641C730C7456}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B17 B25" xr:uid="{2DB65D46-00C2-4C0B-A067-155B441BF7B7}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27" xr:uid="{E31D8AC6-F419-4993-B9DD-AED5034AECBF}">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1498,121 +1560,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9660F2-BB6F-4594-AA8D-C4B63D64351F}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="42"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="42"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="42"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:B5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAFFA4A4-AE14-4748-801F-0FDC1C9F0879}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="42"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="42"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="42"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65FFFCA-880E-4B23-A557-61D090E83602}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removal of unnecessary config after 4G section
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D823F1D-F3F5-46F1-B399-71DA8324D97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C33895F-E9D8-4F2D-998F-6A08DEED7C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,9 +196,6 @@
     <t>backup_DC_Tunnel_Speed</t>
   </si>
   <si>
-    <t>APAC</t>
-  </si>
-  <si>
     <t>This means if you want the zscaler to be configured</t>
   </si>
   <si>
@@ -206,6 +203,9 @@
   </si>
   <si>
     <t>If you select 4G+Cellular to TRUE APN has to be specified.</t>
+  </si>
+  <si>
+    <t>EMEA</t>
   </si>
 </sst>
 </file>
@@ -838,6 +838,21 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -861,21 +876,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1160,7 +1160,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,10 +1172,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="42"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
         <v>16</v>
@@ -1186,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>43</v>
@@ -1204,10 +1204,10 @@
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="39"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="4"/>
       <c r="D4" s="18"/>
     </row>
@@ -1268,10 +1268,10 @@
       <c r="D9" s="21"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="41"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="4"/>
       <c r="D10" s="22"/>
     </row>
@@ -1354,14 +1354,14 @@
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="41"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="4"/>
       <c r="D18" s="22" t="s">
         <v>45</v>
@@ -1424,7 +1424,7 @@
         <v>42</v>
       </c>
       <c r="B24" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>43</v>
@@ -1442,25 +1442,25 @@
       <c r="D25" s="19"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="39"/>
+      <c r="B26" s="44"/>
       <c r="C26" s="4"/>
       <c r="D26" s="32"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="45" t="b">
+      <c r="A27" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="C27" s="46" t="s">
+      <c r="C27" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="43" t="s">
-        <v>56</v>
+      <c r="D27" s="35" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1470,7 +1470,7 @@
       <c r="B28" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="34" t="s">
         <v>43</v>
       </c>
       <c r="D28" s="19"/>
@@ -1496,10 +1496,10 @@
       <c r="D30" s="23"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="35"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="4"/>
       <c r="D31" s="22"/>
     </row>

</xml_diff>

<commit_message>
Filter strings changes, delete line if True for end clearing method.
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C33895F-E9D8-4F2D-998F-6A08DEED7C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B95F76-7BC5-4BA0-A782-E550DA2950C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Info" sheetId="1" r:id="rId1"/>
@@ -1338,7 +1338,7 @@
         <v>42</v>
       </c>
       <c r="B16" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>43</v>
@@ -1424,7 +1424,7 @@
         <v>42</v>
       </c>
       <c r="B24" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
ZBFW while cellular is FALSE fixed.
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B95F76-7BC5-4BA0-A782-E550DA2950C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7ED8B1-5A49-4799-848A-9B4B5D8AD0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1159,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1260,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
cleanup of unnecessary EIGRP and LAN int sections
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7ED8B1-5A49-4799-848A-9B4B5D8AD0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91979659-F999-41BA-890D-79355D293541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -205,7 +205,7 @@
     <t>If you select 4G+Cellular to TRUE APN has to be specified.</t>
   </si>
   <si>
-    <t>EMEA</t>
+    <t>NAM</t>
   </si>
 </sst>
 </file>
@@ -1159,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added IF statemet to run just code which is required for EIGRP and LAN cleanup
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91979659-F999-41BA-890D-79355D293541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5D1E3B-C8DB-42E4-8EBF-F813870A78BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -205,7 +205,7 @@
     <t>If you select 4G+Cellular to TRUE APN has to be specified.</t>
   </si>
   <si>
-    <t>NAM</t>
+    <t>APAC</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1160,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cleanup of content from branch types to cert enroll
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5D1E3B-C8DB-42E4-8EBF-F813870A78BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C47FB3-4804-4E9C-88B3-A8C574025E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="LAN routes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="BASE_SMART_FLOW">'Main Info'!$B$7:$B$8</definedName>
+    <definedName name="BASE_SMART_FLOW">'Main Info'!$B$7:$B$9</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
   <si>
     <t>Region</t>
   </si>
@@ -205,7 +205,10 @@
     <t>If you select 4G+Cellular to TRUE APN has to be specified.</t>
   </si>
   <si>
-    <t>APAC</t>
+    <t>NAM</t>
+  </si>
+  <si>
+    <t>Converged router</t>
   </si>
 </sst>
 </file>
@@ -1157,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,313 +1248,328 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>47</v>
+        <v>59</v>
+      </c>
+      <c r="B8" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>43</v>
       </c>
       <c r="D8" s="20"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="10" t="b">
+      <c r="B10" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C10" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="21"/>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="D10" s="21"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="22"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="B11" s="46"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="22"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="19" t="s">
+      <c r="C12" s="29"/>
+      <c r="D12" s="19" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="20" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="8">
-        <v>100</v>
+        <v>51</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="20" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="B14" s="8">
+        <v>100</v>
       </c>
       <c r="C14" s="30"/>
-      <c r="D14" s="20"/>
+      <c r="D14" s="20" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="8">
         <v>20</v>
       </c>
+      <c r="B15" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="C15" s="30"/>
-      <c r="D15" s="20" t="s">
-        <v>19</v>
-      </c>
+      <c r="D15" s="20"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8">
+        <v>20</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="8" t="b">
+      <c r="B17" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C17" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="20"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B18" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="21" t="s">
+      <c r="C18" s="31"/>
+      <c r="D18" s="21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45" t="s">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="22" t="s">
+      <c r="B19" s="46"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="19" t="s">
+      <c r="C20" s="29"/>
+      <c r="D20" s="19" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="20" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="8">
-        <v>40</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B21" s="8"/>
       <c r="C21" s="30"/>
-      <c r="D21" s="20"/>
+      <c r="D21" s="20" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>27</v>
+        <v>53</v>
+      </c>
+      <c r="B22" s="8">
+        <v>40</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="20"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="8">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="20"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="8">
+        <v>20</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="20"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="8" t="b">
+      <c r="B25" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C25" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="20"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B26" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="19"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="43" t="s">
+      <c r="C26" s="33"/>
+      <c r="D26" s="19"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="32"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="B27" s="44"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="32"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="37" t="b">
+      <c r="B28" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C28" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D28" s="35" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B29" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C29" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="D29" s="19"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B30" s="8">
         <v>50</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
+      <c r="C30" s="30"/>
+      <c r="D30" s="20"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B31" s="13">
         <v>40</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="23"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="39" t="s">
+      <c r="C31" s="28"/>
+      <c r="D31" s="23"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="22"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="B32" s="40"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="22"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B33" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="19"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
+      <c r="C33" s="29"/>
+      <c r="D33" s="19"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B34" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="24"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A27:B27"/>
   </mergeCells>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B7" xr:uid="{6F22417C-AD18-4E4D-B071-70A75C435361}">
       <formula1>"BASE,SMART,FLOW"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B8" xr:uid="{4F4D49CC-A654-4619-9B24-65BC6A1BEBDE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B9" xr:uid="{4F4D49CC-A654-4619-9B24-65BC6A1BEBDE}">
       <formula1>"False, True - New Router, True - Production router"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B9 B16 B24" xr:uid="{40737FED-04A3-4B54-B994-6B1C06BE492C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B10 B17 B25" xr:uid="{40737FED-04A3-4B54-B994-6B1C06BE492C}">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B28" xr:uid="{92AB63BB-4C2D-4BF2-85DE-EF3376E22321}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B29" xr:uid="{92AB63BB-4C2D-4BF2-85DE-EF3376E22321}">
       <formula1>"IPSEC,GRE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B2" xr:uid="{EE08AF00-27BF-4CFF-B4E8-48A38BCB5CAE}">
       <formula1>"APAC,EMEA,NAM"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" prompt="Select the cell to the left to activate the drop-down menu." sqref="C2 C16:C17 C7:C9 C24:C25 C27:C28" xr:uid="{06058C94-713F-44F2-B256-641C730C7456}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B17 B25" xr:uid="{2DB65D46-00C2-4C0B-A067-155B441BF7B7}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27" xr:uid="{E31D8AC6-F419-4993-B9DD-AED5034AECBF}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" prompt="Select the cell to the left to activate the drop-down menu." sqref="C2 C17:C18 C28:C29 C25:C26 C7:C10" xr:uid="{06058C94-713F-44F2-B256-641C730C7456}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B18 B26" xr:uid="{2DB65D46-00C2-4C0B-A067-155B441BF7B7}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28" xr:uid="{E31D8AC6-F419-4993-B9DD-AED5034AECBF}">
       <formula1>"True,False"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="Please set the value from list!" sqref="B8" xr:uid="{D6B27975-02AC-469D-AC0E-AAEE7C516630}">
+      <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Config cleanup based on the Branch Type finished.
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C47FB3-4804-4E9C-88B3-A8C574025E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14E946F-9635-43B9-BD7B-CC6D03AFAB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>Region</t>
   </si>
@@ -64,9 +64,6 @@
     <t>10.173.130.16</t>
   </si>
   <si>
-    <t>BASE</t>
-  </si>
-  <si>
     <t>Main Link</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>Not required if DHCP is used</t>
   </si>
   <si>
-    <t>True - Production router</t>
-  </si>
-  <si>
     <t>APN</t>
   </si>
   <si>
@@ -209,6 +203,12 @@
   </si>
   <si>
     <t>Converged router</t>
+  </si>
+  <si>
+    <t>FLOW</t>
+  </si>
+  <si>
+    <t>Only for NAM - has no effect for the other regions</t>
   </si>
 </sst>
 </file>
@@ -1162,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,7 +1181,7 @@
       <c r="B1" s="42"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1189,10 +1189,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="27"/>
     </row>
@@ -1239,52 +1239,56 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>47</v>
+      <c r="B9" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="20"/>
+        <v>42</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="21"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="46"/>
       <c r="C11" s="4"/>
@@ -1292,121 +1296,121 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="8">
         <v>100</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="20"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="8">
         <v>20</v>
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>42</v>
-      </c>
-      <c r="B17" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>43</v>
       </c>
       <c r="D17" s="20"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="46"/>
       <c r="C19" s="4"/>
       <c r="D19" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="30"/>
       <c r="D21" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B22" s="8">
         <v>40</v>
@@ -1416,17 +1420,17 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="20"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B24" s="8">
         <v>20</v>
@@ -1436,29 +1440,29 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" s="8" t="b">
         <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="20"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" s="33"/>
       <c r="D26" s="19"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="44"/>
       <c r="C27" s="4"/>
@@ -1466,33 +1470,33 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" s="37" t="b">
         <v>1</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>30</v>
-      </c>
       <c r="C29" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" s="19"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="8">
         <v>50</v>
@@ -1502,7 +1506,7 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="13">
         <v>40</v>
@@ -1512,7 +1516,7 @@
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="40"/>
       <c r="C32" s="4"/>
@@ -1520,20 +1524,20 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="19"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="28"/>
       <c r="D34" s="24"/>
@@ -1592,22 +1596,22 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Multiline String check for file beginning cleaup
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14E946F-9635-43B9-BD7B-CC6D03AFAB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A6F571-7020-4FC6-BBB2-6FECC195F3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
   <si>
     <t>Region</t>
   </si>
@@ -199,16 +199,19 @@
     <t>If you select 4G+Cellular to TRUE APN has to be specified.</t>
   </si>
   <si>
+    <t>Converged router</t>
+  </si>
+  <si>
+    <t>Only for NAM - has no effect for the other regions</t>
+  </si>
+  <si>
     <t>NAM</t>
   </si>
   <si>
-    <t>Converged router</t>
-  </si>
-  <si>
-    <t>FLOW</t>
-  </si>
-  <si>
-    <t>Only for NAM - has no effect for the other regions</t>
+    <t>SMART</t>
+  </si>
+  <si>
+    <t>True - Production router</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1166,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1192,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>42</v>
@@ -1239,7 +1242,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>42</v>
@@ -1248,30 +1251,30 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>42</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="b">
-        <v>0</v>
+      <c r="B9" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1279,7 +1282,7 @@
         <v>40</v>
       </c>
       <c r="B10" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>42</v>
@@ -1443,7 +1446,7 @@
         <v>41</v>
       </c>
       <c r="B25" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
base design without tunnels handeled.
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD997B2-BCD0-4EAB-A9E8-9945FB61FD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CD93BB-9EF7-4179-8DD9-80C9674F8302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
   <si>
     <t>Region</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Main_IP+mask</t>
   </si>
   <si>
-    <t>192.1.1.2/24</t>
-  </si>
-  <si>
     <t>172.25.1.1</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>Only for NAM - has no effect for the other regions</t>
   </si>
   <si>
-    <t>SMART</t>
-  </si>
-  <si>
     <t>True - Production router</t>
   </si>
   <si>
@@ -248,6 +242,15 @@
   </si>
   <si>
     <t>EMEA</t>
+  </si>
+  <si>
+    <t>BASE</t>
+  </si>
+  <si>
+    <t>IP or DHCP (ip example 192.168.1.1/29)</t>
+  </si>
+  <si>
+    <t>dhcp</t>
   </si>
 </sst>
 </file>
@@ -891,30 +894,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -924,6 +903,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1207,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,10 +1223,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="40"/>
+      <c r="B1" s="44"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
         <v>15</v>
@@ -1234,10 +1237,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="27"/>
     </row>
@@ -1250,14 +1253,14 @@
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="42"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="4"/>
       <c r="D4" s="18"/>
     </row>
@@ -1270,7 +1273,7 @@
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1288,25 +1291,25 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1314,32 +1317,32 @@
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="21"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="44"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="4"/>
       <c r="D11" s="22"/>
     </row>
@@ -1348,23 +1351,23 @@
         <v>21</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="19" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1384,11 +1387,11 @@
         <v>18</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1400,48 +1403,48 @@
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="8" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>44</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="44"/>
+      <c r="B19" s="48"/>
       <c r="C19" s="4"/>
       <c r="D19" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>14</v>
@@ -1453,178 +1456,178 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="30"/>
       <c r="D21" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="8">
         <v>40</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="8">
         <v>20</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="46"/>
+      <c r="C26" s="38"/>
       <c r="D26" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="48"/>
+      <c r="A27" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="48"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="40"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="35" t="b">
         <v>1</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>28</v>
-      </c>
       <c r="C29" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="8">
         <v>50</v>
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="13">
         <v>40</v>
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="38"/>
+      <c r="A32" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="42"/>
       <c r="C32" s="4"/>
       <c r="D32" s="22"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B34" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="37"/>
+      <c r="D34" s="21" t="s">
         <v>67</v>
-      </c>
-      <c r="C34" s="45"/>
-      <c r="D34" s="21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="28"/>
       <c r="D35" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1681,22 +1684,22 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tu26 issue solution preparations
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CD93BB-9EF7-4179-8DD9-80C9674F8302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E410912C-20B4-44C0-86A2-5946D33243C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,13 +244,13 @@
     <t>EMEA</t>
   </si>
   <si>
-    <t>BASE</t>
-  </si>
-  <si>
     <t>IP or DHCP (ip example 192.168.1.1/29)</t>
   </si>
   <si>
     <t>dhcp</t>
+  </si>
+  <si>
+    <t>SMART</t>
   </si>
 </sst>
 </file>
@@ -1210,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,7 +1291,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>40</v>
@@ -1351,11 +1351,11 @@
         <v>21</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
BASE and Smart int + gw handling
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E410912C-20B4-44C0-86A2-5946D33243C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC65F1EC-DE84-46FE-A251-D9BC3ACE4410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
   <si>
     <t>Region</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Main_DC_Tunnel_Speed</t>
   </si>
   <si>
-    <t>DHCP</t>
-  </si>
-  <si>
     <t>Explanatory notes</t>
   </si>
   <si>
@@ -247,10 +244,16 @@
     <t>IP or DHCP (ip example 192.168.1.1/29)</t>
   </si>
   <si>
-    <t>dhcp</t>
-  </si>
-  <si>
     <t>SMART</t>
+  </si>
+  <si>
+    <t>1.1.1.1/24</t>
+  </si>
+  <si>
+    <t>1.1.1.12</t>
+  </si>
+  <si>
+    <t>2.2.2.2/24</t>
   </si>
 </sst>
 </file>
@@ -1210,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,7 +1232,7 @@
       <c r="B1" s="44"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1237,10 +1240,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="27"/>
     </row>
@@ -1253,7 +1256,7 @@
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1273,7 +1276,7 @@
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1291,25 +1294,25 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1317,24 +1320,24 @@
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="21"/>
     </row>
@@ -1348,26 +1351,26 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>72</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1379,19 +1382,19 @@
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1403,132 +1406,134 @@
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="8" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>43</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="48"/>
       <c r="C19" s="4"/>
       <c r="D19" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="8"/>
+        <v>45</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="C21" s="30"/>
       <c r="D21" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="8">
         <v>40</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" s="8">
         <v>20</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>43</v>
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="48"/>
       <c r="C27" s="39"/>
@@ -1536,59 +1541,59 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="35" t="b">
         <v>1</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>27</v>
-      </c>
       <c r="C29" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="8">
         <v>50</v>
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="13">
         <v>40</v>
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="4"/>
@@ -1596,38 +1601,38 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" s="37"/>
       <c r="D34" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="28"/>
       <c r="D35" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1684,22 +1689,22 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tunnels for SMART design finished.
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC65F1EC-DE84-46FE-A251-D9BC3ACE4410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66D51A2-C32A-4566-AE04-180913FA6134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,9 +172,6 @@
     <t>Backup_port_speed</t>
   </si>
   <si>
-    <t>backup_DC_Tunnel_Speed</t>
-  </si>
-  <si>
     <t>This means if you want the zscaler to be configured</t>
   </si>
   <si>
@@ -238,9 +235,6 @@
     <t>Not required in case of DHCP else the field is mandatory.</t>
   </si>
   <si>
-    <t>EMEA</t>
-  </si>
-  <si>
     <t>IP or DHCP (ip example 192.168.1.1/29)</t>
   </si>
   <si>
@@ -254,6 +248,12 @@
   </si>
   <si>
     <t>2.2.2.2/24</t>
+  </si>
+  <si>
+    <t>Backup_DC_Tunnel_Speed</t>
+  </si>
+  <si>
+    <t>NAM</t>
   </si>
 </sst>
 </file>
@@ -1213,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>39</v>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1294,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>39</v>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="8" t="b">
         <v>1</v>
@@ -1312,7 +1312,7 @@
         <v>39</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1320,13 +1320,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1354,11 +1354,11 @@
         <v>20</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
         <v>39</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1442,7 +1442,7 @@
       <c r="B19" s="48"/>
       <c r="C19" s="4"/>
       <c r="D19" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1450,7 +1450,7 @@
         <v>43</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="19" t="s">
@@ -1462,11 +1462,11 @@
         <v>45</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1490,19 +1490,19 @@
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B24" s="8">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1516,7 +1516,7 @@
         <v>39</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1541,7 +1541,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="35" t="b">
         <v>1</v>
@@ -1550,7 +1550,7 @@
         <v>39</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1564,7 +1564,7 @@
         <v>39</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1608,19 +1608,19 @@
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" s="37"/>
       <c r="D34" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1632,7 +1632,7 @@
       </c>
       <c r="C35" s="28"/>
       <c r="D35" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gitignore updated, order in FLOW config done
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66D51A2-C32A-4566-AE04-180913FA6134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94A019B-C0F7-4428-A161-6826FEC5D99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -238,9 +238,6 @@
     <t>IP or DHCP (ip example 192.168.1.1/29)</t>
   </si>
   <si>
-    <t>SMART</t>
-  </si>
-  <si>
     <t>1.1.1.1/24</t>
   </si>
   <si>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>NAM</t>
+  </si>
+  <si>
+    <t>FLOW</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1214,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>39</v>
@@ -1294,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>39</v>
@@ -1354,7 +1354,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="19" t="s">
@@ -1450,7 +1450,7 @@
         <v>43</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="19" t="s">
@@ -1462,7 +1462,7 @@
         <v>45</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="20" t="s">
@@ -1495,7 +1495,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="8">
         <v>40</v>

</xml_diff>

<commit_message>
flow config half way finished
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94A019B-C0F7-4428-A161-6826FEC5D99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1413227F-EE61-4487-ADAB-91B7CBB19F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,10 +250,10 @@
     <t>Backup_DC_Tunnel_Speed</t>
   </si>
   <si>
-    <t>NAM</t>
-  </si>
-  <si>
     <t>FLOW</t>
+  </si>
+  <si>
+    <t>EMEA</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1214,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>39</v>
@@ -1294,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
flow config function refactor. FLOW wain ip assignment fix
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1413227F-EE61-4487-ADAB-91B7CBB19F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A49DC4D-3F59-4E79-9E80-F5FCEE7B896C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23040" yWindow="2028" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Info" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>Backup Link</t>
   </si>
   <si>
-    <t>192.1.1.1</t>
-  </si>
-  <si>
     <t>Main_IP+mask</t>
   </si>
   <si>
@@ -241,19 +238,22 @@
     <t>1.1.1.1/24</t>
   </si>
   <si>
-    <t>1.1.1.12</t>
-  </si>
-  <si>
     <t>2.2.2.2/24</t>
   </si>
   <si>
     <t>Backup_DC_Tunnel_Speed</t>
   </si>
   <si>
-    <t>FLOW</t>
-  </si>
-  <si>
     <t>EMEA</t>
+  </si>
+  <si>
+    <t>1.1.1.2</t>
+  </si>
+  <si>
+    <t>2.2.2.1</t>
+  </si>
+  <si>
+    <t>SMART</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1214,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,10 +1240,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="27"/>
     </row>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1294,25 +1294,25 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1320,24 +1320,24 @@
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="21"/>
     </row>
@@ -1351,26 +1351,26 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1390,11 +1390,11 @@
         <v>17</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1406,33 +1406,33 @@
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="8" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1442,15 +1442,15 @@
       <c r="B19" s="48"/>
       <c r="C19" s="4"/>
       <c r="D19" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="19" t="s">
@@ -1459,81 +1459,81 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="8">
         <v>40</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B24" s="8">
         <v>40</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="48"/>
       <c r="C27" s="39"/>
@@ -1541,59 +1541,59 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" s="35" t="b">
         <v>1</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>26</v>
-      </c>
       <c r="C29" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="8">
         <v>50</v>
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="13">
         <v>40</v>
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="4"/>
@@ -1601,38 +1601,38 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="37"/>
       <c r="D34" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" s="28"/>
       <c r="D35" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1689,22 +1689,22 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cellular for SMART and FLOW fixed.
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F38077-1C56-49FE-8C3E-4F735E4B2A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B82153-B64A-4CDF-8022-1D50F44686B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -247,13 +247,13 @@
     <t>2.2.2.1</t>
   </si>
   <si>
-    <t>dhcp</t>
-  </si>
-  <si>
     <t>CANnr4003ALEX101</t>
   </si>
   <si>
-    <t>BASE</t>
+    <t>FLOW</t>
+  </si>
+  <si>
+    <t>2.2.2.2/24</t>
   </si>
 </sst>
 </file>
@@ -1213,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,7 +1272,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="19" t="s">
@@ -1294,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>37</v>
@@ -1306,7 +1306,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>37</v>
@@ -1450,7 +1450,7 @@
         <v>41</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="19" t="s">
@@ -1510,7 +1510,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Problem with cellular filtering fixed
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B82153-B64A-4CDF-8022-1D50F44686B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB62589-A098-47EE-8C25-CB31CCAECFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
   <si>
     <t>Region</t>
   </si>
@@ -178,9 +178,6 @@
     <t>Only for NAM - has no effect for the other regions</t>
   </si>
   <si>
-    <t>True - Production router</t>
-  </si>
-  <si>
     <t>Washington, Frankfurt, Singapur ....</t>
   </si>
   <si>
@@ -238,9 +235,6 @@
     <t>Backup_DC_Tunnel_Speed</t>
   </si>
   <si>
-    <t>EMEA</t>
-  </si>
-  <si>
     <t>1.1.1.2</t>
   </si>
   <si>
@@ -250,10 +244,16 @@
     <t>CANnr4003ALEX101</t>
   </si>
   <si>
-    <t>FLOW</t>
-  </si>
-  <si>
     <t>2.2.2.2/24</t>
+  </si>
+  <si>
+    <t>internet.odferky.com</t>
+  </si>
+  <si>
+    <t>BASE</t>
+  </si>
+  <si>
+    <t>NAM</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1214,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>37</v>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1272,11 +1272,11 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1306,7 +1306,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>37</v>
@@ -1319,8 +1319,8 @@
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>49</v>
+      <c r="B9" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>37</v>
@@ -1354,11 +1354,11 @@
         <v>18</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1366,11 +1366,11 @@
         <v>42</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
         <v>37</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1442,7 +1442,7 @@
       <c r="B19" s="48"/>
       <c r="C19" s="4"/>
       <c r="D19" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1450,7 +1450,7 @@
         <v>41</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="19" t="s">
@@ -1462,11 +1462,11 @@
         <v>43</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1490,19 +1490,19 @@
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24" s="8">
         <v>40</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1510,13 +1510,13 @@
         <v>36</v>
       </c>
       <c r="B25" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>37</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1524,11 +1524,11 @@
         <v>39</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1564,7 +1564,7 @@
         <v>37</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1608,19 +1608,19 @@
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="37"/>
       <c r="D34" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1632,7 +1632,7 @@
       </c>
       <c r="C35" s="28"/>
       <c r="D35" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tunnel source for cellular = DONE
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79965174-382C-4769-B875-F5A6E4917632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B878109-6C73-4AFF-9E44-BF445817DB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,10 +250,10 @@
     <t>internet.odferky.com</t>
   </si>
   <si>
-    <t>BASE</t>
-  </si>
-  <si>
     <t>APAC</t>
+  </si>
+  <si>
+    <t>SMART</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1214,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>37</v>
@@ -1294,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>37</v>
@@ -1510,7 +1510,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
APNs need to be fixed
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B878109-6C73-4AFF-9E44-BF445817DB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158DCAED-F8B1-40D7-A635-A138758BD9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1214,7 +1214,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1414,7 @@
         <v>36</v>
       </c>
       <c r="B17" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
INET in cellular needs to be fixed.
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC1B9C1-7053-42E7-80FA-2C922907782A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43817D59-A64C-4820-8317-B3ADF3732425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1213,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
INETs in cellular fixed
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43817D59-A64C-4820-8317-B3ADF3732425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D0E7D9-ACF1-497F-AB63-24DFA6269A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Info" sheetId="1" r:id="rId1"/>
@@ -250,10 +250,10 @@
     <t>internet.odferky.com</t>
   </si>
   <si>
-    <t>APAC</t>
-  </si>
-  <si>
     <t>SMART</t>
+  </si>
+  <si>
+    <t>EMEA</t>
   </si>
 </sst>
 </file>
@@ -1213,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>37</v>
@@ -1294,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>37</v>
@@ -1510,7 +1510,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Cellular finished. APN works Fine now
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D0E7D9-ACF1-497F-AB63-24DFA6269A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9EE960-21BF-41A1-919C-EB8C47F35E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,10 +250,10 @@
     <t>internet.odferky.com</t>
   </si>
   <si>
+    <t>EMEA</t>
+  </si>
+  <si>
     <t>SMART</t>
-  </si>
-  <si>
-    <t>EMEA</t>
   </si>
 </sst>
 </file>
@@ -1213,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>37</v>
@@ -1294,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>37</v>
@@ -1414,7 +1414,7 @@
         <v>36</v>
       </c>
       <c r="B17" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>37</v>
@@ -1510,7 +1510,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
The formating is finished.
</commit_message>
<xml_diff>
--- a/setup.xlsx
+++ b/setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brani\OneDrive\Počítač\DMVPN config\DMVPN_Configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411CBA5E-3740-4D46-B164-95C3748244C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFE3F56-7B5E-4D4D-96A4-62B8BB75BABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1764" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23040" yWindow="2880" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Info" sheetId="1" r:id="rId1"/>
@@ -250,10 +250,10 @@
     <t>SWEnr4003ALEX101</t>
   </si>
   <si>
-    <t>FLOW</t>
-  </si>
-  <si>
     <t>NAM</t>
+  </si>
+  <si>
+    <t>SMART</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1214,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>37</v>
@@ -1294,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>37</v>

</xml_diff>